<commit_message>
SITEWORK-257: updated knolltextiles_info and _approvals data files.
</commit_message>
<xml_diff>
--- a/resources/knolltextiles_info.xlsx
+++ b/resources/knolltextiles_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robcorp/dev/knoll/elf/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC9DEB1F-829A-374B-8F96-03621162C101}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A479CB6-033A-1042-983C-093BD24739C6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4780" yWindow="-23540" windowWidth="38400" windowHeight="23540" xr2:uid="{BAA11FA2-89BB-D24C-A1A7-B81561103F1B}"/>
+    <workbookView xWindow="-4780" yWindow="-23540" windowWidth="38400" windowHeight="23540" xr2:uid="{55734EE2-664A-9545-8E60-3A39DB93993C}"/>
   </bookViews>
   <sheets>
     <sheet name="TextilesInfo" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1298" uniqueCount="682">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="677">
   <si>
     <t>Grade</t>
   </si>
@@ -1863,15 +1863,6 @@
     <t>al-5014-snowshoe.jpg</t>
   </si>
   <si>
-    <t>Amazon</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
     <t>Antique</t>
   </si>
   <si>
@@ -2056,12 +2047,6 @@
   </si>
   <si>
     <t>ss-2256-chalk.jpg</t>
-  </si>
-  <si>
-    <t>blank</t>
-  </si>
-  <si>
-    <t>Z</t>
   </si>
   <si>
     <t>Name</t>
@@ -2165,77 +2150,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
-    <dxf>
-      <font>
-        <color rgb="FFFFC000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFC000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="0.39994506668294322"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFC000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFC000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="0.39994506668294322"/>
-      </font>
-    </dxf>
+  <dxfs count="19">
     <dxf>
       <font>
         <color rgb="FFFFC000"/>
@@ -2489,19 +2404,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{76C0CFFF-DBC1-2F4D-9290-18506F7AA669}" name="Table1" displayName="Table1" ref="A1:G311" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
-  <autoFilter ref="A1:G311" xr:uid="{7513FA51-9AC2-F844-B831-5FE05763A85D}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G311">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3B5BB322-A43A-0146-BF8A-B0252631E6DA}" name="Table1" displayName="Table1" ref="A1:G297" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <autoFilter ref="A1:G297" xr:uid="{7513FA51-9AC2-F844-B831-5FE05763A85D}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G297">
     <sortCondition ref="C2"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{E358A903-F8E3-6047-97CD-F7F8FBC17744}" name="Name" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{12ADD32E-B1FF-DA4E-BBF5-BC50E185836B}" name="PartNum" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{13884A45-6791-0B45-B956-3363F0E01A8D}" name="Grade" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{25052439-5F1A-F44A-83AD-2B164A67698D}" name="EssntlSKUs" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{A3838B46-06B7-534D-A2CF-23685870D5C8}" name="PrimarySKU" dataDxfId="22"/>
-    <tableColumn id="7" xr3:uid="{3135D594-DAEE-294D-AD52-67145F213391}" name="Type" dataDxfId="21"/>
-    <tableColumn id="8" xr3:uid="{F112122F-2492-D843-A0EC-A4C9DE77E696}" name="LeatherImage" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{7E262240-4139-E247-81F3-8D1598553645}" name="Name" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{406ED010-E6F0-4F46-B5DB-0E92C699A2DE}" name="PartNum" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{0B385DC1-B76E-174F-A3F8-8098F99B8878}" name="Grade" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{20A9E80D-DE56-C444-BBDE-96F66E8D1686}" name="EssntlSKUs" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{91445DD5-4C6B-2740-9888-7CC4D9E48EEB}" name="PrimarySKU" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{290B1904-C4E3-B34F-B952-C2DDF783F907}" name="Type" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{36719C63-0CA8-2443-8D06-2D59B03AE6FF}" name="LeatherImage" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2803,12 +2718,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65DE13D6-2101-2649-A860-0E14CCA0A0E3}">
-  <dimension ref="A1:G311"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{867D6400-C000-DF4E-A762-8AD07353319E}">
+  <dimension ref="A1:G297"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G1:G1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2823,25 +2736,25 @@
   <sheetData>
     <row r="1" spans="1:7" ht="74" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>677</v>
+        <v>672</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>678</v>
+        <v>673</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>680</v>
+        <v>675</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>681</v>
+        <v>676</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -8006,29 +7919,29 @@
         <v>629</v>
       </c>
       <c r="C284" s="9" t="s">
-        <v>608</v>
+        <v>630</v>
       </c>
       <c r="F284" s="5" t="s">
         <v>579</v>
       </c>
       <c r="G284" s="5" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
     </row>
     <row r="285" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A285" s="4" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B285" s="4" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="C285" s="9" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="F285" s="5" t="s">
         <v>579</v>
       </c>
-      <c r="G285" s="5" t="s">
+      <c r="G285" s="4" t="s">
         <v>634</v>
       </c>
     </row>
@@ -8040,24 +7953,24 @@
         <v>636</v>
       </c>
       <c r="C286" s="9" t="s">
-        <v>633</v>
+        <v>637</v>
       </c>
       <c r="F286" s="5" t="s">
         <v>579</v>
       </c>
       <c r="G286" s="4" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="287" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A287" s="4" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="B287" s="4" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="C287" s="9" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="F287" s="5" t="s">
         <v>579</v>
@@ -8074,7 +7987,7 @@
         <v>643</v>
       </c>
       <c r="C288" s="9" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="F288" s="5" t="s">
         <v>579</v>
@@ -8091,7 +8004,7 @@
         <v>646</v>
       </c>
       <c r="C289" s="9" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="F289" s="5" t="s">
         <v>579</v>
@@ -8108,7 +8021,7 @@
         <v>649</v>
       </c>
       <c r="C290" s="9" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="F290" s="5" t="s">
         <v>579</v>
@@ -8125,7 +8038,7 @@
         <v>652</v>
       </c>
       <c r="C291" s="9" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="F291" s="5" t="s">
         <v>579</v>
@@ -8142,7 +8055,7 @@
         <v>655</v>
       </c>
       <c r="C292" s="9" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="F292" s="5" t="s">
         <v>579</v>
@@ -8159,7 +8072,7 @@
         <v>658</v>
       </c>
       <c r="C293" s="9" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="F293" s="5" t="s">
         <v>579</v>
@@ -8176,7 +8089,7 @@
         <v>661</v>
       </c>
       <c r="C294" s="9" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="F294" s="5" t="s">
         <v>579</v>
@@ -8193,7 +8106,7 @@
         <v>664</v>
       </c>
       <c r="C295" s="9" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="F295" s="5" t="s">
         <v>579</v>
@@ -8210,7 +8123,7 @@
         <v>667</v>
       </c>
       <c r="C296" s="9" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="F296" s="5" t="s">
         <v>579</v>
@@ -8227,7 +8140,7 @@
         <v>670</v>
       </c>
       <c r="C297" s="9" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="F297" s="5" t="s">
         <v>579</v>
@@ -8236,232 +8149,8 @@
         <v>671</v>
       </c>
     </row>
-    <row r="298" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A298" s="4" t="s">
-        <v>672</v>
-      </c>
-      <c r="B298" s="4" t="s">
-        <v>673</v>
-      </c>
-      <c r="C298" s="9" t="s">
-        <v>640</v>
-      </c>
-      <c r="F298" s="5" t="s">
-        <v>579</v>
-      </c>
-      <c r="G298" s="4" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="299" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A299" s="5" t="s">
-        <v>675</v>
-      </c>
-      <c r="B299" s="5" t="s">
-        <v>611</v>
-      </c>
-      <c r="C299" s="6" t="s">
-        <v>676</v>
-      </c>
-      <c r="F299" s="5"/>
-      <c r="G299" s="5"/>
-    </row>
-    <row r="300" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A300" s="5" t="s">
-        <v>675</v>
-      </c>
-      <c r="B300" s="5" t="s">
-        <v>611</v>
-      </c>
-      <c r="C300" s="6" t="s">
-        <v>676</v>
-      </c>
-      <c r="F300" s="5"/>
-      <c r="G300" s="5"/>
-    </row>
-    <row r="301" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A301" s="5" t="s">
-        <v>675</v>
-      </c>
-      <c r="B301" s="5" t="s">
-        <v>611</v>
-      </c>
-      <c r="C301" s="6" t="s">
-        <v>676</v>
-      </c>
-      <c r="F301" s="5"/>
-      <c r="G301" s="5"/>
-    </row>
-    <row r="302" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A302" s="5" t="s">
-        <v>675</v>
-      </c>
-      <c r="B302" s="5" t="s">
-        <v>611</v>
-      </c>
-      <c r="C302" s="6" t="s">
-        <v>676</v>
-      </c>
-      <c r="F302" s="5"/>
-      <c r="G302" s="5"/>
-    </row>
-    <row r="303" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A303" s="5" t="s">
-        <v>675</v>
-      </c>
-      <c r="B303" s="5" t="s">
-        <v>611</v>
-      </c>
-      <c r="C303" s="6" t="s">
-        <v>676</v>
-      </c>
-      <c r="F303" s="5"/>
-      <c r="G303" s="5"/>
-    </row>
-    <row r="304" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A304" s="5" t="s">
-        <v>675</v>
-      </c>
-      <c r="B304" s="5" t="s">
-        <v>611</v>
-      </c>
-      <c r="C304" s="6" t="s">
-        <v>676</v>
-      </c>
-      <c r="F304" s="5"/>
-      <c r="G304" s="5"/>
-    </row>
-    <row r="305" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A305" s="5" t="s">
-        <v>675</v>
-      </c>
-      <c r="B305" s="5" t="s">
-        <v>611</v>
-      </c>
-      <c r="C305" s="6" t="s">
-        <v>676</v>
-      </c>
-      <c r="F305" s="5"/>
-      <c r="G305" s="5"/>
-    </row>
-    <row r="306" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A306" s="5" t="s">
-        <v>675</v>
-      </c>
-      <c r="B306" s="5" t="s">
-        <v>611</v>
-      </c>
-      <c r="C306" s="6" t="s">
-        <v>676</v>
-      </c>
-      <c r="F306" s="5"/>
-      <c r="G306" s="5"/>
-    </row>
-    <row r="307" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A307" s="5" t="s">
-        <v>675</v>
-      </c>
-      <c r="B307" s="5" t="s">
-        <v>611</v>
-      </c>
-      <c r="C307" s="6" t="s">
-        <v>676</v>
-      </c>
-      <c r="F307" s="5"/>
-      <c r="G307" s="5"/>
-    </row>
-    <row r="308" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A308" s="5" t="s">
-        <v>675</v>
-      </c>
-      <c r="B308" s="5" t="s">
-        <v>611</v>
-      </c>
-      <c r="C308" s="6" t="s">
-        <v>676</v>
-      </c>
-      <c r="F308" s="5"/>
-      <c r="G308" s="5"/>
-    </row>
-    <row r="309" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A309" s="5" t="s">
-        <v>675</v>
-      </c>
-      <c r="B309" s="5" t="s">
-        <v>611</v>
-      </c>
-      <c r="C309" s="6" t="s">
-        <v>676</v>
-      </c>
-      <c r="F309" s="5"/>
-      <c r="G309" s="5"/>
-    </row>
-    <row r="310" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A310" s="5" t="s">
-        <v>675</v>
-      </c>
-      <c r="B310" s="5" t="s">
-        <v>611</v>
-      </c>
-      <c r="C310" s="6" t="s">
-        <v>676</v>
-      </c>
-      <c r="F310" s="5"/>
-      <c r="G310" s="5"/>
-    </row>
-    <row r="311" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A311" s="5" t="s">
-        <v>675</v>
-      </c>
-      <c r="B311" s="5" t="s">
-        <v>611</v>
-      </c>
-      <c r="C311" s="6" t="s">
-        <v>676</v>
-      </c>
-      <c r="F311" s="5"/>
-      <c r="G311" s="5"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:E1 D92:D93 D94:E261 A2:B261 A280:E1048576 D2:E91">
-    <cfRule type="cellIs" dxfId="19" priority="18" operator="equal">
-      <formula>"Limited Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="19" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="20" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:E1 D92:D93 D94:E261 A2:C261 A280:E1048576 D2:E91">
-    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
-      <formula>"Pending"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="17" operator="equal">
-      <formula>"Pending"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A262:E279">
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
-      <formula>"Limited Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A262:E279">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
-      <formula>"Pending"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
-      <formula>"Pending"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G261">
+  <conditionalFormatting sqref="A1:E1 D92:D93 D94:E261 A2:B261 D2:E91 G262:G296 A262:E1048576">
     <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>"Limited Yes"</formula>
     </cfRule>
@@ -8472,7 +8161,7 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G261">
+  <conditionalFormatting sqref="A1:E1 D92:D93 D94:E261 A2:C261 D2:E91 G262:G296 A262:E1048576">
     <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -8480,7 +8169,7 @@
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G262:G297">
+  <conditionalFormatting sqref="G261">
     <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>"Limited Yes"</formula>
     </cfRule>
@@ -8491,7 +8180,7 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G262:G297">
+  <conditionalFormatting sqref="G261">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>

</xml_diff>